<commit_message>
Fix wbs 分担修正 feature
</commit_message>
<xml_diff>
--- a/plan/wbs/teamE_wbs_0806.xlsx
+++ b/plan/wbs/teamE_wbs_0806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fullness.LAPTOP-C0HULFB7.000\Desktop\team-dev-spring-boot-ec\plan\wbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106102FE-4781-44B1-981F-7B1D6CCAF9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C13339F-C27B-4131-BDAC-0CF3072F6CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="書籍情報管理システム" sheetId="1" r:id="rId1"/>
@@ -1094,8 +1094,8 @@
   <dimension ref="A1:AME57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1324,7 +1324,7 @@
         <v>45874</v>
       </c>
       <c r="E9" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F9" s="6">
         <v>45874</v>
@@ -1347,7 +1347,7 @@
         <v>45874</v>
       </c>
       <c r="E10" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F10" s="6">
         <v>45874</v>
@@ -1370,7 +1370,7 @@
         <v>45874</v>
       </c>
       <c r="E11" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F11" s="6">
         <v>45874</v>
@@ -1393,7 +1393,7 @@
         <v>45874</v>
       </c>
       <c r="E12" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F12" s="6">
         <v>45874</v>
@@ -1410,13 +1410,13 @@
         <v>78</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="D13" s="6">
         <v>45874</v>
       </c>
       <c r="E13" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F13" s="6">
         <v>45874</v>
@@ -1439,7 +1439,7 @@
         <v>45874</v>
       </c>
       <c r="E14" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F14" s="6">
         <v>45874</v>
@@ -1462,7 +1462,7 @@
         <v>45874</v>
       </c>
       <c r="E15" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F15" s="6">
         <v>45874</v>
@@ -1485,7 +1485,7 @@
         <v>45874</v>
       </c>
       <c r="E16" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F16" s="6">
         <v>45874</v>
@@ -1508,7 +1508,7 @@
         <v>45874</v>
       </c>
       <c r="E17" s="6">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="F17" s="6">
         <v>45874</v>
@@ -1527,13 +1527,13 @@
         <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="6">
         <v>45875</v>
       </c>
       <c r="E18" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1546,13 +1546,13 @@
         <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D19" s="6">
         <v>45875</v>
       </c>
       <c r="E19" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -1565,13 +1565,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="6">
         <v>45875</v>
       </c>
       <c r="E20" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -1584,13 +1584,13 @@
         <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D21" s="6">
         <v>45875</v>
       </c>
       <c r="E21" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -1603,13 +1603,13 @@
         <v>34</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D22" s="6">
         <v>45875</v>
       </c>
       <c r="E22" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -1622,13 +1622,13 @@
         <v>35</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" s="6">
         <v>45875</v>
       </c>
       <c r="E23" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -1641,13 +1641,13 @@
         <v>36</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D24" s="6">
         <v>45875</v>
       </c>
       <c r="E24" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -1660,13 +1660,13 @@
         <v>37</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" s="6">
         <v>45875</v>
       </c>
       <c r="E25" s="6">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -1706,7 +1706,7 @@
         <v>41</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D27" s="6">
         <v>45888</v>
@@ -1725,7 +1725,7 @@
         <v>42</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D28" s="6">
         <v>45888</v>
@@ -1744,7 +1744,7 @@
         <v>43</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D29" s="6">
         <v>45888</v>
@@ -1763,7 +1763,7 @@
         <v>44</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D30" s="6">
         <v>45888</v>
@@ -1782,7 +1782,7 @@
         <v>45</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D31" s="6">
         <v>45888</v>
@@ -1801,7 +1801,7 @@
         <v>46</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D32" s="6">
         <v>45888</v>
@@ -1820,7 +1820,7 @@
         <v>47</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D33" s="6">
         <v>45888</v>
@@ -1839,7 +1839,7 @@
         <v>48</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D34" s="6">
         <v>45888</v>
@@ -1898,13 +1898,13 @@
         <v>52</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D37" s="6">
-        <v>45876</v>
+        <v>45889</v>
       </c>
       <c r="E37" s="6">
-        <v>45876</v>
+        <v>45890</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -1917,13 +1917,13 @@
         <v>53</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D38" s="6">
-        <v>45876</v>
+        <v>45889</v>
       </c>
       <c r="E38" s="6">
-        <v>45876</v>
+        <v>45890</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -1936,13 +1936,13 @@
         <v>54</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D39" s="6">
-        <v>45876</v>
+        <v>45889</v>
       </c>
       <c r="E39" s="6">
-        <v>45876</v>
+        <v>45890</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -1955,13 +1955,13 @@
         <v>55</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D40" s="6">
-        <v>45876</v>
+        <v>45889</v>
       </c>
       <c r="E40" s="6">
-        <v>45876</v>
+        <v>45890</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -1974,13 +1974,13 @@
         <v>56</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D41" s="6">
-        <v>45877</v>
+        <v>45889</v>
       </c>
       <c r="E41" s="6">
-        <v>45877</v>
+        <v>45890</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -1993,13 +1993,13 @@
         <v>57</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D42" s="6">
-        <v>45877</v>
+        <v>45889</v>
       </c>
       <c r="E42" s="6">
-        <v>45877</v>
+        <v>45890</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -2012,13 +2012,13 @@
         <v>58</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D43" s="6">
-        <v>45877</v>
+        <v>45889</v>
       </c>
       <c r="E43" s="6">
-        <v>45877</v>
+        <v>45890</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2031,13 +2031,13 @@
         <v>59</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D44" s="6">
-        <v>45877</v>
+        <v>45889</v>
       </c>
       <c r="E44" s="6">
-        <v>45877</v>
+        <v>45890</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -2065,13 +2065,13 @@
         <v>61</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D46" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E46" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2083,13 +2083,13 @@
         <v>62</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D47" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E47" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -2102,13 +2102,13 @@
         <v>63</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D48" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E48" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -2121,13 +2121,13 @@
         <v>64</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D49" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E49" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -2140,13 +2140,13 @@
         <v>65</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D50" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E50" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -2159,13 +2159,13 @@
         <v>66</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D51" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E51" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -2178,13 +2178,13 @@
         <v>67</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D52" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E52" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -2197,13 +2197,13 @@
         <v>68</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D53" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="E53" s="6">
-        <v>45889</v>
+        <v>45891</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -2234,10 +2234,10 @@
         <v>15</v>
       </c>
       <c r="D55" s="6">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="E55" s="6">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>

</xml_diff>